<commit_message>
made corrections to interface selector
</commit_message>
<xml_diff>
--- a/DC1_intf_selectors.xlsx
+++ b/DC1_intf_selectors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tyscott\iac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A402D36B-60E1-4661-A441-73625695D45A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0DF584-217A-4FE9-8C0A-6BB1D5D28F80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="803" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="4140" windowWidth="28800" windowHeight="15540" tabRatio="803" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dc1-spine101" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="293">
   <si>
     <t>dc1-spine101 Interface Selectors</t>
   </si>
@@ -908,6 +908,9 @@
   </si>
   <si>
     <t>lacp_Active</t>
+  </si>
+  <si>
+    <t>port-channel</t>
   </si>
 </sst>
 </file>
@@ -1409,7 +1412,7 @@
       <selection activeCell="F4" sqref="F4:M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -1423,7 +1426,7 @@
     <col min="13" max="13" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1440,7 +1443,7 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="7" t="s">
         <v>1</v>
@@ -1457,7 +1460,7 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1498,7 +1501,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1514,32 +1517,16 @@
       <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="I4" s="2">
-        <v>1</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="L4" s="2">
-        <v>1</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1555,32 +1542,16 @@
       <c r="E5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="I5" s="3">
-        <v>1</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="L5" s="3">
-        <v>1</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -1596,28 +1567,16 @@
       <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>267</v>
-      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="L6" s="2">
-        <v>995</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -1633,28 +1592,16 @@
       <c r="E7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>267</v>
-      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="L7" s="3">
-        <v>995</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -1670,30 +1617,16 @@
       <c r="E8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>266</v>
-      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="2">
-        <v>5</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="L8" s="2">
-        <v>1</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1709,30 +1642,16 @@
       <c r="E9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>266</v>
-      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="3">
-        <v>5</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="L9" s="3">
-        <v>1</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1748,30 +1667,16 @@
       <c r="E10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>266</v>
-      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="2">
-        <v>7</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="L10" s="2">
-        <v>187</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -1787,30 +1692,16 @@
       <c r="E11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>266</v>
-      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="3">
-        <v>7</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="L11" s="3">
-        <v>1</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1826,30 +1717,16 @@
       <c r="E12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>266</v>
-      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="2">
-        <v>9</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="L12" s="2">
-        <v>1</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -1865,30 +1742,16 @@
       <c r="E13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>266</v>
-      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="3">
-        <v>9</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="L13" s="3">
-        <v>1</v>
-      </c>
-      <c r="M13" s="3">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1904,30 +1767,16 @@
       <c r="E14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>266</v>
-      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="2">
-        <v>9</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="L14" s="2">
-        <v>1</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -1943,30 +1792,16 @@
       <c r="E15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>266</v>
-      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="3">
-        <v>9</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="L15" s="3">
-        <v>1</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+    </row>
+    <row r="16" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1982,30 +1817,16 @@
       <c r="E16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>266</v>
-      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="2">
-        <v>13</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="L16" s="2">
-        <v>1</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -2021,30 +1842,16 @@
       <c r="E17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>266</v>
-      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="3">
-        <v>13</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="L17" s="3">
-        <v>1</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -2069,7 +1876,7 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
@@ -2094,7 +1901,7 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
@@ -2119,7 +1926,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
@@ -2144,7 +1951,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
@@ -2169,7 +1976,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>15</v>
       </c>
@@ -2194,7 +2001,7 @@
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>15</v>
       </c>
@@ -2219,7 +2026,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>15</v>
       </c>
@@ -2244,7 +2051,7 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>15</v>
       </c>
@@ -2269,7 +2076,7 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>15</v>
       </c>
@@ -2294,7 +2101,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>15</v>
       </c>
@@ -2319,7 +2126,7 @@
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>15</v>
       </c>
@@ -2344,7 +2151,7 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
@@ -2369,7 +2176,7 @@
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
     </row>
-    <row r="31" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>15</v>
       </c>
@@ -2394,7 +2201,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>15</v>
       </c>
@@ -2419,7 +2226,7 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>15</v>
       </c>
@@ -2444,7 +2251,7 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>15</v>
       </c>
@@ -2469,7 +2276,7 @@
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
     </row>
-    <row r="35" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>15</v>
       </c>
@@ -2494,7 +2301,7 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
     </row>
-    <row r="36" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>15</v>
       </c>
@@ -2519,7 +2326,7 @@
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
     </row>
-    <row r="37" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>15</v>
       </c>
@@ -2544,7 +2351,7 @@
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>15</v>
       </c>
@@ -2569,7 +2376,7 @@
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
     </row>
-    <row r="39" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>15</v>
       </c>
@@ -2594,7 +2401,7 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>15</v>
       </c>
@@ -2619,7 +2426,7 @@
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
     </row>
-    <row r="41" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>15</v>
       </c>
@@ -2644,7 +2451,7 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>15</v>
       </c>
@@ -2669,7 +2476,7 @@
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
     </row>
-    <row r="43" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>15</v>
       </c>
@@ -2694,7 +2501,7 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>15</v>
       </c>
@@ -2719,7 +2526,7 @@
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
     </row>
-    <row r="45" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>15</v>
       </c>
@@ -2744,7 +2551,7 @@
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>15</v>
       </c>
@@ -2769,7 +2576,7 @@
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
     </row>
-    <row r="47" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>15</v>
       </c>
@@ -2794,7 +2601,7 @@
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
     </row>
-    <row r="48" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>15</v>
       </c>
@@ -2819,7 +2626,7 @@
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
     </row>
-    <row r="49" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>15</v>
       </c>
@@ -2844,7 +2651,7 @@
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>15</v>
       </c>
@@ -2869,7 +2676,7 @@
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
     </row>
-    <row r="51" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>15</v>
       </c>
@@ -2894,7 +2701,7 @@
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
     </row>
-    <row r="52" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>15</v>
       </c>
@@ -2919,7 +2726,7 @@
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
     </row>
-    <row r="53" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>15</v>
       </c>
@@ -2944,7 +2751,7 @@
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>15</v>
       </c>
@@ -2969,7 +2776,7 @@
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
     </row>
-    <row r="55" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>15</v>
       </c>
@@ -2994,7 +2801,7 @@
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
     </row>
-    <row r="56" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>15</v>
       </c>
@@ -3019,7 +2826,7 @@
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
     </row>
-    <row r="57" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>15</v>
       </c>
@@ -3044,7 +2851,7 @@
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
     </row>
-    <row r="58" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>15</v>
       </c>
@@ -3069,7 +2876,7 @@
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
     </row>
-    <row r="59" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>15</v>
       </c>
@@ -3094,7 +2901,7 @@
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
     </row>
-    <row r="60" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>15</v>
       </c>
@@ -3119,7 +2926,7 @@
       <c r="L60" s="2"/>
       <c r="M60" s="2"/>
     </row>
-    <row r="61" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>15</v>
       </c>
@@ -3144,7 +2951,7 @@
       <c r="L61" s="3"/>
       <c r="M61" s="3"/>
     </row>
-    <row r="62" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>15</v>
       </c>
@@ -3169,7 +2976,7 @@
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
     </row>
-    <row r="63" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>15</v>
       </c>
@@ -3194,7 +3001,7 @@
       <c r="L63" s="3"/>
       <c r="M63" s="3"/>
     </row>
-    <row r="64" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>15</v>
       </c>
@@ -3219,7 +3026,7 @@
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
     </row>
-    <row r="65" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>15</v>
       </c>
@@ -3244,7 +3051,7 @@
       <c r="L65" s="3"/>
       <c r="M65" s="3"/>
     </row>
-    <row r="66" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>15</v>
       </c>
@@ -3269,7 +3076,7 @@
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
     </row>
-    <row r="67" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>15</v>
       </c>
@@ -3294,7 +3101,7 @@
       <c r="L67" s="3"/>
       <c r="M67" s="3"/>
     </row>
-    <row r="68" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>15</v>
       </c>
@@ -3319,7 +3126,7 @@
       <c r="L68" s="2"/>
       <c r="M68" s="2"/>
     </row>
-    <row r="69" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>15</v>
       </c>
@@ -3344,7 +3151,7 @@
       <c r="L69" s="3"/>
       <c r="M69" s="3"/>
     </row>
-    <row r="70" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>15</v>
       </c>
@@ -3369,7 +3176,7 @@
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
     </row>
-    <row r="71" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>15</v>
       </c>
@@ -3394,7 +3201,7 @@
       <c r="L71" s="3"/>
       <c r="M71" s="3"/>
     </row>
-    <row r="72" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>15</v>
       </c>
@@ -3419,7 +3226,7 @@
       <c r="L72" s="2"/>
       <c r="M72" s="2"/>
     </row>
-    <row r="73" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
         <v>15</v>
       </c>
@@ -3444,7 +3251,7 @@
       <c r="L73" s="3"/>
       <c r="M73" s="3"/>
     </row>
-    <row r="74" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>15</v>
       </c>
@@ -3469,7 +3276,7 @@
       <c r="L74" s="2"/>
       <c r="M74" s="2"/>
     </row>
-    <row r="75" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>15</v>
       </c>
@@ -3494,7 +3301,7 @@
       <c r="L75" s="3"/>
       <c r="M75" s="3"/>
     </row>
-    <row r="76" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>15</v>
       </c>
@@ -3519,7 +3326,7 @@
       <c r="L76" s="2"/>
       <c r="M76" s="2"/>
     </row>
-    <row r="77" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
         <v>15</v>
       </c>
@@ -3544,7 +3351,7 @@
       <c r="L77" s="3"/>
       <c r="M77" s="3"/>
     </row>
-    <row r="78" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>15</v>
       </c>
@@ -3569,7 +3376,7 @@
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
     </row>
-    <row r="79" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>15</v>
       </c>
@@ -3594,7 +3401,7 @@
       <c r="L79" s="3"/>
       <c r="M79" s="3"/>
     </row>
-    <row r="80" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>15</v>
       </c>
@@ -3619,7 +3426,7 @@
       <c r="L80" s="2"/>
       <c r="M80" s="2"/>
     </row>
-    <row r="81" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>15</v>
       </c>
@@ -3644,7 +3451,7 @@
       <c r="L81" s="3"/>
       <c r="M81" s="3"/>
     </row>
-    <row r="82" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>15</v>
       </c>
@@ -3669,7 +3476,7 @@
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
     </row>
-    <row r="83" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>15</v>
       </c>
@@ -3694,7 +3501,7 @@
       <c r="L83" s="3"/>
       <c r="M83" s="3"/>
     </row>
-    <row r="84" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
         <v>15</v>
       </c>
@@ -3719,7 +3526,7 @@
       <c r="L84" s="2"/>
       <c r="M84" s="2"/>
     </row>
-    <row r="85" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
         <v>15</v>
       </c>
@@ -3744,7 +3551,7 @@
       <c r="L85" s="3"/>
       <c r="M85" s="3"/>
     </row>
-    <row r="86" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
         <v>15</v>
       </c>
@@ -3769,7 +3576,7 @@
       <c r="L86" s="2"/>
       <c r="M86" s="2"/>
     </row>
-    <row r="87" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
         <v>15</v>
       </c>
@@ -3794,7 +3601,7 @@
       <c r="L87" s="3"/>
       <c r="M87" s="3"/>
     </row>
-    <row r="88" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
         <v>15</v>
       </c>
@@ -3819,7 +3626,7 @@
       <c r="L88" s="2"/>
       <c r="M88" s="2"/>
     </row>
-    <row r="89" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
         <v>15</v>
       </c>
@@ -3844,7 +3651,7 @@
       <c r="L89" s="3"/>
       <c r="M89" s="3"/>
     </row>
-    <row r="90" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>15</v>
       </c>
@@ -3869,7 +3676,7 @@
       <c r="L90" s="2"/>
       <c r="M90" s="2"/>
     </row>
-    <row r="91" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
         <v>15</v>
       </c>
@@ -3894,7 +3701,7 @@
       <c r="L91" s="3"/>
       <c r="M91" s="3"/>
     </row>
-    <row r="92" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
         <v>15</v>
       </c>
@@ -3919,7 +3726,7 @@
       <c r="L92" s="2"/>
       <c r="M92" s="2"/>
     </row>
-    <row r="93" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
         <v>15</v>
       </c>
@@ -3944,7 +3751,7 @@
       <c r="L93" s="3"/>
       <c r="M93" s="3"/>
     </row>
-    <row r="94" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>15</v>
       </c>
@@ -3969,7 +3776,7 @@
       <c r="L94" s="2"/>
       <c r="M94" s="2"/>
     </row>
-    <row r="95" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
         <v>15</v>
       </c>
@@ -3994,7 +3801,7 @@
       <c r="L95" s="3"/>
       <c r="M95" s="3"/>
     </row>
-    <row r="96" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
         <v>15</v>
       </c>
@@ -4019,7 +3826,7 @@
       <c r="L96" s="2"/>
       <c r="M96" s="2"/>
     </row>
-    <row r="97" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
         <v>15</v>
       </c>
@@ -4044,7 +3851,7 @@
       <c r="L97" s="3"/>
       <c r="M97" s="3"/>
     </row>
-    <row r="98" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
         <v>15</v>
       </c>
@@ -4069,7 +3876,7 @@
       <c r="L98" s="2"/>
       <c r="M98" s="2"/>
     </row>
-    <row r="99" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
         <v>15</v>
       </c>
@@ -4094,7 +3901,7 @@
       <c r="L99" s="3"/>
       <c r="M99" s="3"/>
     </row>
-    <row r="100" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
         <v>15</v>
       </c>
@@ -4119,7 +3926,7 @@
       <c r="L100" s="2"/>
       <c r="M100" s="2"/>
     </row>
-    <row r="101" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
         <v>15</v>
       </c>
@@ -4144,7 +3951,7 @@
       <c r="L101" s="3"/>
       <c r="M101" s="3"/>
     </row>
-    <row r="102" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
         <v>15</v>
       </c>
@@ -4169,7 +3976,7 @@
       <c r="L102" s="2"/>
       <c r="M102" s="2"/>
     </row>
-    <row r="103" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
         <v>15</v>
       </c>
@@ -4218,11 +4025,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:M17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -4233,10 +4040,10 @@
     <col min="9" max="9" width="15" customWidth="1"/>
     <col min="10" max="10" width="30" customWidth="1"/>
     <col min="11" max="12" width="20" customWidth="1"/>
-    <col min="13" max="13" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>217</v>
       </c>
@@ -4253,7 +4060,7 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="7" t="s">
         <v>1</v>
@@ -4270,7 +4077,7 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -4311,7 +4118,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -4352,7 +4159,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -4372,7 +4179,7 @@
         <v>265</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>266</v>
+        <v>292</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>291</v>
@@ -4393,7 +4200,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -4430,7 +4237,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -4467,7 +4274,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -4508,7 +4315,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -4549,7 +4356,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -4590,7 +4397,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -4631,7 +4438,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -4672,7 +4479,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -4713,7 +4520,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -4754,7 +4561,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -4795,7 +4602,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -4836,7 +4643,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -4877,7 +4684,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -4902,7 +4709,7 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
@@ -4927,7 +4734,7 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
@@ -4952,7 +4759,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
@@ -4977,7 +4784,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
@@ -5002,7 +4809,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>15</v>
       </c>
@@ -5027,7 +4834,7 @@
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>15</v>
       </c>
@@ -5052,7 +4859,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>15</v>
       </c>
@@ -5077,7 +4884,7 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>15</v>
       </c>
@@ -5102,7 +4909,7 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>15</v>
       </c>
@@ -5127,7 +4934,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>15</v>
       </c>
@@ -5152,7 +4959,7 @@
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>15</v>
       </c>
@@ -5177,7 +4984,7 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
@@ -5202,7 +5009,7 @@
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
     </row>
-    <row r="31" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>15</v>
       </c>
@@ -5227,7 +5034,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>15</v>
       </c>
@@ -5252,7 +5059,7 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>15</v>
       </c>
@@ -5277,7 +5084,7 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>15</v>
       </c>
@@ -5302,7 +5109,7 @@
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
     </row>
-    <row r="35" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>15</v>
       </c>
@@ -5327,7 +5134,7 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
     </row>
-    <row r="36" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>15</v>
       </c>
@@ -5352,7 +5159,7 @@
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
     </row>
-    <row r="37" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>15</v>
       </c>
@@ -5377,7 +5184,7 @@
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>15</v>
       </c>
@@ -5402,7 +5209,7 @@
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
     </row>
-    <row r="39" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>15</v>
       </c>
@@ -5427,7 +5234,7 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>15</v>
       </c>
@@ -5452,7 +5259,7 @@
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
     </row>
-    <row r="41" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>15</v>
       </c>
@@ -5477,7 +5284,7 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>15</v>
       </c>
@@ -5502,7 +5309,7 @@
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
     </row>
-    <row r="43" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>15</v>
       </c>
@@ -5527,7 +5334,7 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>15</v>
       </c>
@@ -5552,7 +5359,7 @@
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
     </row>
-    <row r="45" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>15</v>
       </c>
@@ -5577,7 +5384,7 @@
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>15</v>
       </c>
@@ -5602,7 +5409,7 @@
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
     </row>
-    <row r="47" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>15</v>
       </c>
@@ -5627,7 +5434,7 @@
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
     </row>
-    <row r="48" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>15</v>
       </c>
@@ -5652,7 +5459,7 @@
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
     </row>
-    <row r="49" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>15</v>
       </c>
@@ -5677,7 +5484,7 @@
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>15</v>
       </c>
@@ -5702,7 +5509,7 @@
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
     </row>
-    <row r="51" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>15</v>
       </c>
@@ -5727,7 +5534,7 @@
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
     </row>
-    <row r="52" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>15</v>
       </c>
@@ -5752,7 +5559,7 @@
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
     </row>
-    <row r="53" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>15</v>
       </c>
@@ -5777,7 +5584,7 @@
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>15</v>
       </c>
@@ -5802,7 +5609,7 @@
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
     </row>
-    <row r="55" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>15</v>
       </c>
@@ -5827,7 +5634,7 @@
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
     </row>
-    <row r="56" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>15</v>
       </c>
@@ -5852,7 +5659,7 @@
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
     </row>
-    <row r="57" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>15</v>
       </c>
@@ -5882,7 +5689,7 @@
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="B2:M2"/>
   </mergeCells>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A4:A57" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"intf_selector"</formula1>
     </dataValidation>
@@ -5892,6 +5699,7 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H4:H57" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"lacp_Active,lacp_MacPin,lacp_Passive,lacp_Static"</formula1>
     </dataValidation>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4" xr:uid="{F9CB3433-69D4-4769-8123-01A913E9E23A}"/>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5901,11 +5709,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -5916,10 +5724,10 @@
     <col min="9" max="9" width="15" customWidth="1"/>
     <col min="10" max="10" width="30" customWidth="1"/>
     <col min="11" max="12" width="20" customWidth="1"/>
-    <col min="13" max="13" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>263</v>
       </c>
@@ -5936,7 +5744,7 @@
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
     </row>
-    <row r="2" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="7" t="s">
         <v>1</v>
@@ -5953,7 +5761,7 @@
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -5994,7 +5802,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -6035,7 +5843,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -6076,7 +5884,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -6113,7 +5921,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -6150,7 +5958,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -6191,7 +5999,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -6232,7 +6040,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -6273,7 +6081,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -6314,7 +6122,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -6355,7 +6163,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -6396,7 +6204,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -6437,7 +6245,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -6478,7 +6286,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -6519,7 +6327,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -6560,7 +6368,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -6585,7 +6393,7 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
@@ -6610,7 +6418,7 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
@@ -6635,7 +6443,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
@@ -6660,7 +6468,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
@@ -6685,7 +6493,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>15</v>
       </c>
@@ -6710,7 +6518,7 @@
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>15</v>
       </c>
@@ -6735,7 +6543,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>15</v>
       </c>
@@ -6760,7 +6568,7 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>15</v>
       </c>
@@ -6785,7 +6593,7 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>15</v>
       </c>
@@ -6810,7 +6618,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>15</v>
       </c>
@@ -6835,7 +6643,7 @@
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>15</v>
       </c>
@@ -6860,7 +6668,7 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
@@ -6885,7 +6693,7 @@
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
     </row>
-    <row r="31" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>15</v>
       </c>
@@ -6910,7 +6718,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>15</v>
       </c>
@@ -6935,7 +6743,7 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>15</v>
       </c>
@@ -6960,7 +6768,7 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>15</v>
       </c>
@@ -6985,7 +6793,7 @@
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
     </row>
-    <row r="35" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>15</v>
       </c>
@@ -7010,7 +6818,7 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
     </row>
-    <row r="36" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>15</v>
       </c>
@@ -7035,7 +6843,7 @@
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
     </row>
-    <row r="37" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>15</v>
       </c>
@@ -7060,7 +6868,7 @@
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>15</v>
       </c>
@@ -7085,7 +6893,7 @@
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
     </row>
-    <row r="39" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>15</v>
       </c>
@@ -7110,7 +6918,7 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>15</v>
       </c>
@@ -7135,7 +6943,7 @@
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
     </row>
-    <row r="41" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>15</v>
       </c>
@@ -7160,7 +6968,7 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>15</v>
       </c>
@@ -7185,7 +6993,7 @@
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
     </row>
-    <row r="43" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>15</v>
       </c>
@@ -7210,7 +7018,7 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>15</v>
       </c>
@@ -7235,7 +7043,7 @@
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
     </row>
-    <row r="45" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>15</v>
       </c>
@@ -7260,7 +7068,7 @@
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>15</v>
       </c>
@@ -7285,7 +7093,7 @@
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
     </row>
-    <row r="47" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>15</v>
       </c>
@@ -7310,7 +7118,7 @@
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
     </row>
-    <row r="48" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>15</v>
       </c>
@@ -7335,7 +7143,7 @@
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
     </row>
-    <row r="49" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>15</v>
       </c>
@@ -7360,7 +7168,7 @@
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>15</v>
       </c>
@@ -7385,7 +7193,7 @@
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
     </row>
-    <row r="51" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>15</v>
       </c>
@@ -7410,7 +7218,7 @@
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
     </row>
-    <row r="52" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>15</v>
       </c>
@@ -7435,7 +7243,7 @@
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
     </row>
-    <row r="53" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>15</v>
       </c>
@@ -7460,7 +7268,7 @@
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>15</v>
       </c>
@@ -7485,7 +7293,7 @@
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
     </row>
-    <row r="55" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>15</v>
       </c>
@@ -7510,7 +7318,7 @@
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
     </row>
-    <row r="56" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>15</v>
       </c>
@@ -7535,7 +7343,7 @@
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
     </row>
-    <row r="57" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
adding best practices variablel support
</commit_message>
<xml_diff>
--- a/DC1_intf_selectors.xlsx
+++ b/DC1_intf_selectors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tyscott\iac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B6AECF-865F-47DD-9A28-40EEC41F75F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FCFA8A-6CDD-4B07-B013-A5A94BD2E193}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="4140" windowWidth="28800" windowHeight="15540" tabRatio="803" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="803" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dc1-spine101" sheetId="1" r:id="rId1"/>
@@ -1065,18 +1065,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="2" xfId="5">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="6">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="2" xfId="5">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="6">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1431,40 +1431,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
+      <c r="B2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -4335,7 +4335,7 @@
   <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:N17"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4348,44 +4348,44 @@
     <col min="10" max="10" width="15" customWidth="1"/>
     <col min="11" max="11" width="30" customWidth="1"/>
     <col min="12" max="13" width="20" customWidth="1"/>
-    <col min="14" max="14" width="30" customWidth="1"/>
+    <col min="14" max="14" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
+      <c r="B2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -4450,28 +4450,28 @@
       <c r="F4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="J4" s="8">
-        <v>1</v>
-      </c>
-      <c r="K4" s="8" t="s">
+      <c r="J4" s="5">
+        <v>1</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="M4" s="8">
-        <v>1</v>
-      </c>
-      <c r="N4" s="8" t="s">
+      <c r="M4" s="5">
+        <v>1</v>
+      </c>
+      <c r="N4" s="5" t="s">
         <v>271</v>
       </c>
     </row>
@@ -4494,28 +4494,28 @@
       <c r="F5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="J5" s="9">
-        <v>1</v>
-      </c>
-      <c r="K5" s="9" t="s">
+      <c r="J5" s="6">
+        <v>1</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="L5" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="M5" s="9">
-        <v>1</v>
-      </c>
-      <c r="N5" s="9" t="s">
+      <c r="M5" s="6">
+        <v>1</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>271</v>
       </c>
     </row>
@@ -4538,24 +4538,24 @@
       <c r="F6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8" t="s">
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="5">
         <v>995</v>
       </c>
-      <c r="N6" s="8"/>
+      <c r="N6" s="5"/>
     </row>
     <row r="7" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
@@ -4576,24 +4576,24 @@
       <c r="F7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9" t="s">
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="L7" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="6">
         <v>995</v>
       </c>
-      <c r="N7" s="9"/>
+      <c r="N7" s="6"/>
     </row>
     <row r="8" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
@@ -4614,28 +4614,28 @@
       <c r="F8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="5">
         <v>5</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="L8" s="8" t="s">
+      <c r="L8" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="M8" s="8">
-        <v>1</v>
-      </c>
-      <c r="N8" s="8"/>
+      <c r="M8" s="5">
+        <v>1</v>
+      </c>
+      <c r="N8" s="5"/>
     </row>
     <row r="9" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
@@ -4656,28 +4656,28 @@
       <c r="F9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="6">
         <v>5</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="L9" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="M9" s="9">
-        <v>1</v>
-      </c>
-      <c r="N9" s="9"/>
+      <c r="M9" s="6">
+        <v>1</v>
+      </c>
+      <c r="N9" s="6"/>
     </row>
     <row r="10" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
@@ -4698,28 +4698,28 @@
       <c r="F10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="5">
         <v>7</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="L10" s="8" t="s">
+      <c r="L10" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="M10" s="8">
+      <c r="M10" s="5">
         <v>187</v>
       </c>
-      <c r="N10" s="8"/>
+      <c r="N10" s="5"/>
     </row>
     <row r="11" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
@@ -4740,28 +4740,28 @@
       <c r="F11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="6">
         <v>7</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="K11" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="L11" s="9" t="s">
+      <c r="L11" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="M11" s="9">
-        <v>1</v>
-      </c>
-      <c r="N11" s="9" t="s">
+      <c r="M11" s="6">
+        <v>1</v>
+      </c>
+      <c r="N11" s="6" t="s">
         <v>282</v>
       </c>
     </row>
@@ -4784,28 +4784,28 @@
       <c r="F12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="5">
         <v>9</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="L12" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="M12" s="8">
-        <v>1</v>
-      </c>
-      <c r="N12" s="8" t="s">
+      <c r="M12" s="5">
+        <v>1</v>
+      </c>
+      <c r="N12" s="5" t="s">
         <v>282</v>
       </c>
     </row>
@@ -4828,28 +4828,28 @@
       <c r="F13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="6">
         <v>9</v>
       </c>
-      <c r="K13" s="9" t="s">
+      <c r="K13" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="L13" s="9" t="s">
+      <c r="L13" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="M13" s="9">
-        <v>1</v>
-      </c>
-      <c r="N13" s="9">
+      <c r="M13" s="6">
+        <v>1</v>
+      </c>
+      <c r="N13" s="6">
         <v>64</v>
       </c>
     </row>
@@ -4872,28 +4872,28 @@
       <c r="F14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="5">
         <v>9</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="K14" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="L14" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="M14" s="8">
-        <v>1</v>
-      </c>
-      <c r="N14" s="8" t="s">
+      <c r="M14" s="5">
+        <v>1</v>
+      </c>
+      <c r="N14" s="5" t="s">
         <v>286</v>
       </c>
     </row>
@@ -4916,28 +4916,28 @@
       <c r="F15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="H15" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="6">
         <v>9</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="K15" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="L15" s="9" t="s">
+      <c r="L15" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="M15" s="9">
-        <v>1</v>
-      </c>
-      <c r="N15" s="9" t="s">
+      <c r="M15" s="6">
+        <v>1</v>
+      </c>
+      <c r="N15" s="6" t="s">
         <v>286</v>
       </c>
     </row>
@@ -4960,28 +4960,28 @@
       <c r="F16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="J16" s="8">
+      <c r="J16" s="5">
         <v>13</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="K16" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="L16" s="8" t="s">
+      <c r="L16" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="M16" s="8">
-        <v>1</v>
-      </c>
-      <c r="N16" s="8" t="s">
+      <c r="M16" s="5">
+        <v>1</v>
+      </c>
+      <c r="N16" s="5" t="s">
         <v>290</v>
       </c>
     </row>
@@ -5004,28 +5004,28 @@
       <c r="F17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="H17" s="9" t="s">
+      <c r="H17" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="I17" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="6">
         <v>13</v>
       </c>
-      <c r="K17" s="9" t="s">
+      <c r="K17" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="L17" s="9" t="s">
+      <c r="L17" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="M17" s="9">
-        <v>1</v>
-      </c>
-      <c r="N17" s="9" t="s">
+      <c r="M17" s="6">
+        <v>1</v>
+      </c>
+      <c r="N17" s="6" t="s">
         <v>290</v>
       </c>
     </row>
@@ -6174,7 +6174,7 @@
   <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:N17"/>
+      <selection activeCell="N4" sqref="N4:N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6187,44 +6187,44 @@
     <col min="10" max="10" width="15" customWidth="1"/>
     <col min="11" max="11" width="30" customWidth="1"/>
     <col min="12" max="13" width="20" customWidth="1"/>
-    <col min="14" max="14" width="30" customWidth="1"/>
+    <col min="14" max="14" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
     </row>
     <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
+      <c r="B2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -6289,28 +6289,28 @@
       <c r="F4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="J4" s="8">
-        <v>1</v>
-      </c>
-      <c r="K4" s="8" t="s">
+      <c r="J4" s="5">
+        <v>1</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="M4" s="8">
-        <v>1</v>
-      </c>
-      <c r="N4" s="8" t="s">
+      <c r="M4" s="5">
+        <v>1</v>
+      </c>
+      <c r="N4" s="5" t="s">
         <v>271</v>
       </c>
     </row>
@@ -6333,28 +6333,28 @@
       <c r="F5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="J5" s="9">
-        <v>1</v>
-      </c>
-      <c r="K5" s="9" t="s">
+      <c r="J5" s="6">
+        <v>1</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="L5" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="M5" s="9">
-        <v>1</v>
-      </c>
-      <c r="N5" s="9" t="s">
+      <c r="M5" s="6">
+        <v>1</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>271</v>
       </c>
     </row>
@@ -6377,24 +6377,24 @@
       <c r="F6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8" t="s">
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="5">
         <v>995</v>
       </c>
-      <c r="N6" s="8"/>
+      <c r="N6" s="5"/>
     </row>
     <row r="7" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
@@ -6415,24 +6415,24 @@
       <c r="F7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9" t="s">
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="L7" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="6">
         <v>995</v>
       </c>
-      <c r="N7" s="9"/>
+      <c r="N7" s="6"/>
     </row>
     <row r="8" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
@@ -6453,28 +6453,28 @@
       <c r="F8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="5">
         <v>5</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="L8" s="8" t="s">
+      <c r="L8" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="M8" s="8">
-        <v>1</v>
-      </c>
-      <c r="N8" s="8"/>
+      <c r="M8" s="5">
+        <v>1</v>
+      </c>
+      <c r="N8" s="5"/>
     </row>
     <row r="9" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
@@ -6495,28 +6495,28 @@
       <c r="F9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="6">
         <v>5</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="L9" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="M9" s="9">
-        <v>1</v>
-      </c>
-      <c r="N9" s="9"/>
+      <c r="M9" s="6">
+        <v>1</v>
+      </c>
+      <c r="N9" s="6"/>
     </row>
     <row r="10" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
@@ -6537,28 +6537,28 @@
       <c r="F10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="5">
         <v>7</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="L10" s="8" t="s">
+      <c r="L10" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="M10" s="8">
+      <c r="M10" s="5">
         <v>187</v>
       </c>
-      <c r="N10" s="8"/>
+      <c r="N10" s="5"/>
     </row>
     <row r="11" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
@@ -6579,28 +6579,28 @@
       <c r="F11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="6">
         <v>7</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="K11" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="L11" s="9" t="s">
+      <c r="L11" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="M11" s="9">
-        <v>1</v>
-      </c>
-      <c r="N11" s="9" t="s">
+      <c r="M11" s="6">
+        <v>1</v>
+      </c>
+      <c r="N11" s="6" t="s">
         <v>282</v>
       </c>
     </row>
@@ -6623,28 +6623,28 @@
       <c r="F12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="5">
         <v>9</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="L12" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="M12" s="8">
-        <v>1</v>
-      </c>
-      <c r="N12" s="8" t="s">
+      <c r="M12" s="5">
+        <v>1</v>
+      </c>
+      <c r="N12" s="5" t="s">
         <v>282</v>
       </c>
     </row>
@@ -6667,28 +6667,28 @@
       <c r="F13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="6">
         <v>9</v>
       </c>
-      <c r="K13" s="9" t="s">
+      <c r="K13" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="L13" s="9" t="s">
+      <c r="L13" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="M13" s="9">
-        <v>1</v>
-      </c>
-      <c r="N13" s="9">
+      <c r="M13" s="6">
+        <v>1</v>
+      </c>
+      <c r="N13" s="6">
         <v>64</v>
       </c>
     </row>
@@ -6711,28 +6711,28 @@
       <c r="F14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="5">
         <v>9</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="K14" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="L14" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="M14" s="8">
-        <v>1</v>
-      </c>
-      <c r="N14" s="8" t="s">
+      <c r="M14" s="5">
+        <v>1</v>
+      </c>
+      <c r="N14" s="5" t="s">
         <v>286</v>
       </c>
     </row>
@@ -6755,28 +6755,28 @@
       <c r="F15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="H15" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="6">
         <v>9</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="K15" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="L15" s="9" t="s">
+      <c r="L15" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="M15" s="9">
-        <v>1</v>
-      </c>
-      <c r="N15" s="9" t="s">
+      <c r="M15" s="6">
+        <v>1</v>
+      </c>
+      <c r="N15" s="6" t="s">
         <v>286</v>
       </c>
     </row>
@@ -6799,28 +6799,28 @@
       <c r="F16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="J16" s="8">
+      <c r="J16" s="5">
         <v>13</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="K16" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="L16" s="8" t="s">
+      <c r="L16" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="M16" s="8">
-        <v>1</v>
-      </c>
-      <c r="N16" s="8" t="s">
+      <c r="M16" s="5">
+        <v>1</v>
+      </c>
+      <c r="N16" s="5" t="s">
         <v>290</v>
       </c>
     </row>
@@ -6843,28 +6843,28 @@
       <c r="F17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="H17" s="9" t="s">
+      <c r="H17" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="I17" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="6">
         <v>13</v>
       </c>
-      <c r="K17" s="9" t="s">
+      <c r="K17" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="L17" s="9" t="s">
+      <c r="L17" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="M17" s="9">
-        <v>1</v>
-      </c>
-      <c r="N17" s="9" t="s">
+      <c r="M17" s="6">
+        <v>1</v>
+      </c>
+      <c r="N17" s="6" t="s">
         <v>290</v>
       </c>
     </row>

</xml_diff>

<commit_message>
scripts are broken right now.  pending update
</commit_message>
<xml_diff>
--- a/DC1_intf_selectors.xlsx
+++ b/DC1_intf_selectors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tyscott\iac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FCFA8A-6CDD-4B07-B013-A5A94BD2E193}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CBF368-40E3-47EF-BC54-4D4613177956}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="803" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="803" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dc1-spine101" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="293">
   <si>
     <t>dc1-spine101 Interface Selectors</t>
   </si>
@@ -910,6 +910,9 @@
   </si>
   <si>
     <t>asgard-leaf102-Eth1/50</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -1414,7 +1417,7 @@
   <dimension ref="A1:N103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:N1"/>
+      <selection activeCell="A4" sqref="A4:N53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4334,8 +4337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4623,8 +4626,8 @@
       <c r="I8" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="J8" s="5">
-        <v>5</v>
+      <c r="J8" s="5" t="s">
+        <v>292</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>278</v>
@@ -6173,7 +6176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N4" sqref="N4:N17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
getting close to finishing up
</commit_message>
<xml_diff>
--- a/DC1_intf_selectors.xlsx
+++ b/DC1_intf_selectors.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tyscott\iac\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\tyscott\iac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A221B05E-E3F6-4F97-B95E-1B502BBA9B8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B51FB1-13B1-4378-8C5C-3F0AC5F62957}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="803" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="803" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dc1-spine101" sheetId="1" r:id="rId1"/>
@@ -1413,7 +1413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
@@ -4332,8 +4332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:I57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Just about to Publish version 0.5 of the project
</commit_message>
<xml_diff>
--- a/DC1_intf_selectors.xlsx
+++ b/DC1_intf_selectors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\tyscott\iac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B51FB1-13B1-4378-8C5C-3F0AC5F62957}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{916133B3-89E6-4916-9EB3-0ED0D7827781}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="803" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4333,7 +4333,7 @@
   <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>